<commit_message>
can import excel 80% progress
</commit_message>
<xml_diff>
--- a/public/DataRekapitulasi/tester2.xlsx
+++ b/public/DataRekapitulasi/tester2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BeaCukai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E898D32-EAF2-454B-A22F-00D362828371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A5679A-4CED-4E0D-A59F-14EBD6DE0954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77CDF6BC-62B1-454B-BA68-4693489A40FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Kanwil DJBC Jawa Tengah dan D.I. Yogyakarta</t>
   </si>
@@ -80,10 +80,7 @@
     <t>ada</t>
   </si>
   <si>
-    <t>add</t>
-  </si>
-  <si>
-    <t>dd</t>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -190,7 +187,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -245,7 +242,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -300,7 +297,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -355,7 +352,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -410,7 +407,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -465,7 +462,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -520,7 +517,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -575,7 +572,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -630,7 +627,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -685,7 +682,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -740,7 +737,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -795,7 +792,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -850,7 +847,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -905,7 +902,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -960,7 +957,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1015,7 +1012,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1070,7 +1067,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1125,7 +1122,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1180,7 +1177,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1235,7 +1232,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1290,7 +1287,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1345,7 +1342,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1400,7 +1397,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1455,7 +1452,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1510,7 +1507,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1565,7 +1562,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1620,7 +1617,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1675,7 +1672,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1730,7 +1727,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1785,7 +1782,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1840,7 +1837,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2213,82 +2210,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171DEBAF-6943-41BE-8172-A84E3905FD19}">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AM1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.5546875" customWidth="1"/>
-    <col min="2" max="2" width="61.5546875" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="33.21875" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
-    <col min="14" max="14" width="89" customWidth="1"/>
-    <col min="23" max="23" width="21.21875" customWidth="1"/>
-    <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="32" max="32" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="61.5546875" customWidth="1"/>
+    <col min="2" max="2" width="56.77734375" customWidth="1"/>
+    <col min="3" max="3" width="33.21875" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" customWidth="1"/>
+    <col min="11" max="11" width="19.44140625" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="89" customWidth="1"/>
+    <col min="22" max="22" width="21.21875" customWidth="1"/>
+    <col min="23" max="23" width="16" customWidth="1"/>
+    <col min="30" max="30" width="26" customWidth="1"/>
+    <col min="31" max="31" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:39" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>45680</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>45680</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2">
+        <v>45680</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2">
-        <v>45680</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2">
-        <v>45680</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2">
-        <v>45680</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -2297,65 +2299,56 @@
       <c r="U1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="6">
+        <f>AB1*1485</f>
+        <v>326700</v>
+      </c>
+      <c r="W1" s="6">
+        <f t="shared" ref="W1" si="0">AB1*746</f>
+        <v>164120</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="W1" s="6">
-        <f t="shared" ref="W1" si="0">AC1*1485</f>
-        <v>326700</v>
-      </c>
-      <c r="X1" s="6">
-        <f t="shared" ref="X1" si="1">AC1*746</f>
-        <v>164120</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA1" s="1">
+      <c r="Z1" s="1">
         <v>39</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AC1" s="7">
+      <c r="AB1" s="7">
         <v>220</v>
       </c>
+      <c r="AC1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="AD1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AF1" s="2">
-        <f>I1</f>
+      <c r="AE1" s="2">
+        <f>H1</f>
         <v>45680</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>15</v>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AN1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
big testing excel done
</commit_message>
<xml_diff>
--- a/public/DataRekapitulasi/tester2.xlsx
+++ b/public/DataRekapitulasi/tester2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BeaCukai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A5679A-4CED-4E0D-A59F-14EBD6DE0954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAEDDFC-E72B-4B22-8274-4AC67D24BC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77CDF6BC-62B1-454B-BA68-4693489A40FA}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{77CDF6BC-62B1-454B-BA68-4693489A40FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Kanwil DJBC Jawa Tengah dan D.I. Yogyakarta</t>
   </si>
@@ -81,6 +81,117 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>SBP No</t>
+  </si>
+  <si>
+    <t>Kantor</t>
+  </si>
+  <si>
+    <t>SBP Tgl</t>
+  </si>
+  <si>
+    <t>LP/LP1 No</t>
+  </si>
+  <si>
+    <t>LP/LP1 Tgl</t>
+  </si>
+  <si>
+    <t>SPLIT No</t>
+  </si>
+  <si>
+    <t>SPLIT Tgl</t>
+  </si>
+  <si>
+    <t>Jenis Pelanggaran</t>
+  </si>
+  <si>
+    <t>Nama Pelanggar</t>
+  </si>
+  <si>
+    <t>NIK/NPWP</t>
+  </si>
+  <si>
+    <t>Alternatif Penyelesaian Masalah</t>
+  </si>
+  <si>
+    <t>Pasal yang dilanggar</t>
+  </si>
+  <si>
+    <t>No LK</t>
+  </si>
+  <si>
+    <t>SPTP No</t>
+  </si>
+  <si>
+    <t>SPTP Tgl</t>
+  </si>
+  <si>
+    <t>SPDP No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPDP Tgl </t>
+  </si>
+  <si>
+    <t>Nama TSK</t>
+  </si>
+  <si>
+    <t>Status Proses</t>
+  </si>
+  <si>
+    <t>Perkiraan Nilai Barang</t>
+  </si>
+  <si>
+    <t>Potensi Kehilangan Penerimaan Negara</t>
+  </si>
+  <si>
+    <t>Nama Pengguna Jasa</t>
+  </si>
+  <si>
+    <t>NPWP Pengguna Jasa</t>
+  </si>
+  <si>
+    <t>Kode Komoditi</t>
+  </si>
+  <si>
+    <t>Jenis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumlah </t>
+  </si>
+  <si>
+    <t>Satuan</t>
+  </si>
+  <si>
+    <t>BA Pencacahan No</t>
+  </si>
+  <si>
+    <t>BA Pencacahan Tgl</t>
+  </si>
+  <si>
+    <t>Kep BDN No</t>
+  </si>
+  <si>
+    <t>Kep BMN Tgl</t>
+  </si>
+  <si>
+    <t>Kep BDN Tgl</t>
+  </si>
+  <si>
+    <t>Kep BMN No</t>
+  </si>
+  <si>
+    <t>Tap Sita No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap Sita Tgl </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>proses</t>
   </si>
 </sst>
 </file>
@@ -189,7 +300,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -244,7 +355,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -299,7 +410,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -354,7 +465,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -409,7 +520,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -464,7 +575,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -519,7 +630,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -574,7 +685,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -629,7 +740,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -684,7 +795,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -739,7 +850,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -794,7 +905,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -849,7 +960,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -904,7 +1015,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -959,7 +1070,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1014,7 +1125,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1069,7 +1180,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1124,7 +1235,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1179,7 +1290,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1234,7 +1345,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1289,7 +1400,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1344,7 +1455,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1399,7 +1510,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1454,7 +1565,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1509,7 +1620,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1564,7 +1675,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1619,7 +1730,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1674,7 +1785,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1729,7 +1840,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1784,7 +1895,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -1839,7 +1950,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="247650"/>
@@ -2210,15 +2321,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171DEBAF-6943-41BE-8172-A84E3905FD19}">
-  <dimension ref="A1:AM1"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="56.77734375" customWidth="1"/>
     <col min="3" max="3" width="33.21875" customWidth="1"/>
     <col min="4" max="4" width="25.21875" customWidth="1"/>
@@ -2229,125 +2340,259 @@
     <col min="9" max="9" width="23" customWidth="1"/>
     <col min="10" max="10" width="21.5546875" customWidth="1"/>
     <col min="11" max="11" width="19.44140625" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="12" max="12" width="29.77734375" customWidth="1"/>
     <col min="13" max="13" width="89" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" customWidth="1"/>
+    <col min="20" max="20" width="11.77734375" customWidth="1"/>
+    <col min="21" max="21" width="12.44140625" customWidth="1"/>
     <col min="22" max="22" width="21.21875" customWidth="1"/>
-    <col min="23" max="23" width="16" customWidth="1"/>
+    <col min="23" max="23" width="34.77734375" customWidth="1"/>
+    <col min="24" max="24" width="18.44140625" customWidth="1"/>
+    <col min="25" max="25" width="24.21875" customWidth="1"/>
+    <col min="26" max="26" width="13.44140625" customWidth="1"/>
     <col min="30" max="30" width="26" customWidth="1"/>
     <col min="31" max="31" width="19.5546875" customWidth="1"/>
+    <col min="32" max="32" width="17.21875" customWidth="1"/>
+    <col min="33" max="33" width="14.77734375" customWidth="1"/>
+    <col min="34" max="34" width="13.44140625" customWidth="1"/>
+    <col min="35" max="35" width="14.5546875" customWidth="1"/>
+    <col min="36" max="36" width="12.6640625" customWidth="1"/>
+    <col min="37" max="37" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:39" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D2" s="2">
         <v>45680</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F2" s="2">
         <v>45680</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H2" s="2">
         <v>45680</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="6">
-        <f>AB1*1485</f>
+      <c r="V2" s="6">
+        <f>AB2*1485</f>
         <v>326700</v>
       </c>
-      <c r="W1" s="6">
-        <f t="shared" ref="W1" si="0">AB1*746</f>
+      <c r="W2" s="6">
+        <f t="shared" ref="W2" si="0">AB2*746</f>
         <v>164120</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Z2" s="1">
         <v>39</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="7">
+      <c r="AB2" s="7">
         <v>220</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AE1" s="2">
-        <f>H1</f>
+      <c r="AE2" s="2">
+        <f>H2</f>
         <v>45680</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="1" t="s">
+      <c r="AG2" s="2">
+        <v>45681</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="1" t="s">
+      <c r="AI2" s="2">
+        <v>45680</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="1" t="s">
+      <c r="AK2" s="2">
+        <v>45684</v>
+      </c>
+      <c r="AL2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>